<commit_message>
:sparkles: Finished sample functions, sample labeler
</commit_message>
<xml_diff>
--- a/docs/moralmachine-data-description.xlsx
+++ b/docs/moralmachine-data-description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steed/heuristic-moral-machine/data/moralmachine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{82F3B168-7019-DE42-8674-19AE864A0F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{98733A1E-455B-B646-BEA0-FE226514A007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="660" windowWidth="28040" windowHeight="17040"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="99" uniqueCount="74">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="110" uniqueCount="84">
   <si>
     <t>Moral Machine Data</t>
   </si>
@@ -72,18 +72,12 @@
     <t xml:space="preserve">'Intervention' </t>
   </si>
   <si>
-    <t>whether the user intervened to divert the car? always 0</t>
-  </si>
-  <si>
     <t xml:space="preserve">'PedPed' </t>
   </si>
   <si>
     <t>binary</t>
   </si>
   <si>
-    <t>0 means "passengers vs. pedestrians"; 1 means "pedestrians vs. pedestrians"</t>
-  </si>
-  <si>
     <t xml:space="preserve">'Barrier' </t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t xml:space="preserve">'AttributeLevel' </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">'ScenarioTypeStrict' </t>
   </si>
   <si>
@@ -195,9 +186,6 @@
     <t xml:space="preserve">'Cat </t>
   </si>
   <si>
-    <t xml:space="preserve"> what factor(s) differ between scenarios</t>
-  </si>
-  <si>
     <t>binary? Only 0's in 2000</t>
   </si>
   <si>
@@ -207,9 +195,6 @@
     <t>[1, 13]</t>
   </si>
   <si>
-    <t>which scenario in the 13-scenario session is being viewed (1st, 2nd, etc.)</t>
-  </si>
-  <si>
     <t>Binary, some NaN</t>
   </si>
   <si>
@@ -234,19 +219,64 @@
     <t>[0, 1]</t>
   </si>
   <si>
-    <t>Whether the user saved this set of characters</t>
-  </si>
-  <si>
     <t>('Desktop', 'Mobile', nan)</t>
   </si>
   <si>
-    <t>3 letter country abbrv</t>
-  </si>
-  <si>
-    <t>[0, 2]</t>
-  </si>
-  <si>
-    <t>[0, 5]</t>
+    <t>[0, 5], some NaN</t>
+  </si>
+  <si>
+    <t>0 means a test of "passengers vs. pedestrians"; 1 means a test of  "pedestrians vs. pedestrians" (i.e. two sets of pedestrians in the street, probably empty car)</t>
+  </si>
+  <si>
+    <t>Whether the car hits the barrier in this scenario?</t>
+  </si>
+  <si>
+    <t>targeted difference between scenarios</t>
+  </si>
+  <si>
+    <t>Which attribute level this scenario represents</t>
+  </si>
+  <si>
+    <t>Whether this scenario was presented on the left hand side</t>
+  </si>
+  <si>
+    <t>Whether the user saved the passengers (or pedestrians) in this scenario</t>
+  </si>
+  <si>
+    <t>which scenario in the 13-scenario session is being viewed (1st, 2nd, etc.)?</t>
+  </si>
+  <si>
+    <t>whether or not this scenario requires the user to intervene (swerve)</t>
+  </si>
+  <si>
+    <t>the nondefault choice</t>
+  </si>
+  <si>
+    <t>the default choice</t>
+  </si>
+  <si>
+    <t>true if rand, I think</t>
+  </si>
+  <si>
+    <t>total # of characters in this scenario</t>
+  </si>
+  <si>
+    <t>difference from the alternative</t>
+  </si>
+  <si>
+    <t>where this was taken (why does this matter?)</t>
+  </si>
+  <si>
+    <t>with respect to the pedestrians, 0 means "no legality", as in there is no crossing light; 1 means explicitly legal (green light); 2 means explicitly illegal (red light)</t>
+  </si>
+  <si>
+    <t>Whether the description for this scenario was shown in the GUI</t>
+  </si>
+  <si>
+    <t>The user's country</t>
+  </si>
+  <si>
+    <t>&gt;200 3-letter country abbrvs</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1121,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1137,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -1148,7 +1178,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -1159,7 +1189,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1170,10 +1200,10 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1181,313 +1211,346 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>31</v>
+      <c r="A24" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>